<commit_message>
Correct assignment of two Gerris IDs
</commit_message>
<xml_diff>
--- a/inst/extdata/interface/outlet_conversion.xlsx
+++ b/inst/extdata/interface/outlet_conversion.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20371"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20387"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mzamzo\Desktop\server_austausch\R_interface\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mzamzo\Documents\R\git\kwb.misa\inst\extdata\interface\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B561414-11B5-4963-B5ED-09E252219C9D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D4DB09-1D61-40FB-AD91-A14E2CB12067}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2506,8 +2506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3344,10 +3344,10 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>439</v>
@@ -3383,15 +3383,15 @@
         <v>41</v>
       </c>
       <c r="N21" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>538</v>
@@ -3427,7 +3427,7 @@
         <v>41</v>
       </c>
       <c r="N22" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.35">

</xml_diff>